<commit_message>
Minor cleanups, and updated README file.
</commit_message>
<xml_diff>
--- a/adsorbentSheet.xlsx
+++ b/adsorbentSheet.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N5"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>896</v>
+        <v>588.25</v>
       </c>
       <c r="C2">
         <v>6.8</v>

</xml_diff>